<commit_message>
updating mapping sheet for SID
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Arrest_Query_Request_Service/artifacts/service_model/information_model/Arrest_Query_Request_IEPD/documentation/arrest_query_request_mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Arrest_Query_Request_Service/artifacts/service_model/information_model/Arrest_Query_Request_IEPD/documentation/arrest_query_request_mapping.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="26925" windowHeight="10365"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="26920" windowHeight="10360"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -88,7 +93,7 @@
     <t>Person State Identification Number (SID)</t>
   </si>
   <si>
-    <t>/aqrequest:ArrestQueryRequest/nc:PersonStateIdentification/nc:IdentificationID</t>
+    <t>/aqrequest:ArrestQueryRequest/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -1095,23 +1100,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="126.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="145.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="126.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="145.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="62.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="45" hidden="1" customHeight="1">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1121,13 +1126,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="13"/>
       <c r="C2" s="20"/>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="18">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1139,7 +1144,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="18" customFormat="1" ht="18">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1152,7 @@
       <c r="C4" s="11"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:4" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="22" customFormat="1" ht="18">
       <c r="A5" s="23" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1164,7 @@
       </c>
       <c r="D5" s="24"/>
     </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="16" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
@@ -1171,7 +1176,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="16" customFormat="1">
       <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +1188,7 @@
       </c>
       <c r="D7" s="19"/>
     </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="16" customFormat="1">
       <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
@@ -1195,7 +1200,7 @@
       </c>
       <c r="D8" s="19"/>
     </row>
-    <row r="9" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="16" customFormat="1">
       <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
@@ -1207,7 +1212,7 @@
       </c>
       <c r="D9" s="19"/>
     </row>
-    <row r="10" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="16" customFormat="1">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1220,7 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1227,207 +1232,207 @@
       </c>
       <c r="D11" s="25"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="3"/>
       <c r="B12" s="14"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="14"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="3"/>
       <c r="B14" s="14"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="3"/>
       <c r="B15" s="14"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="3"/>
       <c r="B16" s="14"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="14"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="14"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="14"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="14"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="14"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="14"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="14"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="14"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="14"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="14"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="14"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="14"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="3"/>
       <c r="B29" s="14"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="14"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="14"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="14"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="3"/>
       <c r="B33" s="14"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="14"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="14"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="14"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="3"/>
       <c r="B37" s="14"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="14"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="3"/>
       <c r="B39" s="14"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="3"/>
       <c r="B40" s="14"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="14"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="3"/>
       <c r="B42" s="14"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="14"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="14"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="3"/>
       <c r="B45" s="14"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="3"/>
       <c r="B46" s="14"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="3"/>
       <c r="B47" s="14"/>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="3"/>
       <c r="B48" s="14"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="3"/>
       <c r="B49" s="14"/>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="3"/>
       <c r="B50" s="14"/>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="3"/>
       <c r="B51" s="14"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="3"/>
       <c r="B52" s="14"/>
       <c r="C52" s="4"/>
@@ -1437,6 +1442,11 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>